<commit_message>
y bus function completed
</commit_message>
<xml_diff>
--- a/gauss_seidel_method/example_6.8/ex_impedence_data_3_bus.xlsx
+++ b/gauss_seidel_method/example_6.8/ex_impedence_data_3_bus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28060" windowHeight="11040"/>
+    <workbookView windowWidth="28060" windowHeight="11060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
-  <si>
-    <t>No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
   <si>
     <t>Bus</t>
   </si>
@@ -34,9 +31,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -47,6 +44,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -56,24 +60,48 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -85,6 +113,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -93,15 +128,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -109,83 +145,44 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,13 +197,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +293,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,37 +305,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,115 +371,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,15 +402,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,6 +445,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -471,168 +488,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -960,35 +957,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="B1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A1" sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="2:5">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:5">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1002,10 +993,7 @@
         <v>0.025</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
+    <row r="3" spans="2:5">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1019,10 +1007,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
+    <row r="4" spans="2:5">
       <c r="B4">
         <v>2</v>
       </c>

</xml_diff>